<commit_message>
feat: detecting trend changes
</commit_message>
<xml_diff>
--- a/renko_pseudoalgorithm.xlsx
+++ b/renko_pseudoalgorithm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\renko-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -185,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,22 +714,22 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E19" s="9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F19" s="9">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G19" s="9">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>